<commit_message>
Added final Diary entry Santhiya_Nagarajan
</commit_message>
<xml_diff>
--- a/diaries/diary-Santhiya-Nagarajan.xlsx
+++ b/diaries/diary-Santhiya-Nagarajan.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="192">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -518,6 +518,84 @@
   </si>
   <si>
     <t>Feeling good!</t>
+  </si>
+  <si>
+    <t>Looking forward to the guest speakers and discussing questions based on design patterns</t>
+  </si>
+  <si>
+    <t>We started the discussion of pull request and it was interesting to hear different stories. We learnt three more KEP. Finally, we learned about testing by using JPacman. In the end, we had super excited two guests.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We learned about the different ideas behind various test cases written in JPacman. Many a times, I was confused about the use of mock when we can achieve the results normally, should go through mockito basics once more. StartUpTest was written in a different format and was basic in nature. Glad end to end testing was mentioned in the lecture, I believe our Pull request had to make a few adjustments regarding that testing. Finally, we had guests who were super enthusiastic and in a way intimidating. It was great to see the drive they have in learning new languages and they made sure to keep us engaged throughout the lecture. It was great to see frequency and amplitude modulation all over again after the physics course couple of years back. The activity made us think in all areas right from the programming language similarities to Software Architecture design of Pipe and Filter. Hope one day we are as excited about our careers as they are! </t>
+  </si>
+  <si>
+    <t>Enthusiastic! Glad that the homework is not due next week.</t>
+  </si>
+  <si>
+    <t>20:00 - 21:00</t>
+  </si>
+  <si>
+    <t>To discuss the test cases for the pull request we had submitted</t>
+  </si>
+  <si>
+    <t>We finished the discussion on the test cases and were able to come up with rough concepts to be covered in the new test</t>
+  </si>
+  <si>
+    <t>As we were asked to write different test cases, we looked into the preexisting cases and whether we could add the test cases. We also realized that the functionality we added can be tested on its own in a different class and hence we moved forward with this idea.</t>
+  </si>
+  <si>
+    <t>Feeling confused!</t>
+  </si>
+  <si>
+    <t>Looking forward to the final lecture, I guess we will have a lot of key value points to take home.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We finished discussion about pull requests again. None of the teams had worked on the new assignment and hence were not able to review that. Glad that we are on the same boat. We learnt three new KEP. We watched interesting history videos and visualization techniques utilized commonly. Finally, we went over the attitude. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Looking forward to apply the KEP in real life. Upon watching a few history videos, I realized how pointless certain media can be unless the context is well explained or relevant. Nevertheless it was beautiful to look at. Enjoyed the git log and git blame functionalities. Moving on to visualization, I liked the feature where it showed connectivity among different developers to know who you have to interact with the most. Finally, going over the attitude helps us understand the importance of maintaining a good reputation among our colleagues. </t>
+  </si>
+  <si>
+    <t>Tired!</t>
+  </si>
+  <si>
+    <t>18:00 - 20:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To discuss the report on addressing the issue of tooltip </t>
+  </si>
+  <si>
+    <t>We finished writing the report on the ToolTip.</t>
+  </si>
+  <si>
+    <t>Upon getting active feedbacks from the developers, we were able to quickly grasp the intent behind their comments and were able to incorporate the changes rather quickly. We feel happy that we had such active developers and they were very welcoming to new comers we believe!</t>
+  </si>
+  <si>
+    <t>Happy!</t>
+  </si>
+  <si>
+    <t>To finalize the report on the initial pull request and come up with three existing test cases that are potentially interesting</t>
+  </si>
+  <si>
+    <t>We finished writing up the report for initial pull request. We finalized on four existing test classes that we would like to cover</t>
+  </si>
+  <si>
+    <t xml:space="preserve">While writing the test cases and hence submitting, we realized the importance of coding style, even though logically we have made firm contributions, the lack of format makes our Pull request yet to be merged. Anyway, we are happy we were bale to identify the essence and modify and I am sure in a few days we will be able to fix the coding style. </t>
+  </si>
+  <si>
+    <t>20:00 - 00:00</t>
+  </si>
+  <si>
+    <t>To finish up the report on existing test cases and make final submission</t>
+  </si>
+  <si>
+    <t>We are glad that we are done with all the assignments and that this is the last diary entry.</t>
+  </si>
+  <si>
+    <t>In the end of this, we have definitely learned how to document effectively. We saw how our writings changed over the course of these ten weeks in order to get the point across to Kaj. The initial low scores have motivated us to work hard in earning higher scores in the end. In terms  of technical knowledge, we were happy that even with limited knowledge we were able to contribute and make fruitful conversations with the developers to contribute to a reference management tool that is being use in great meany universities’ libraries. Hearing other people’s stories have of course restored our faith in luck, having such active community is what helped us to move through the pull request and issues confidently. Finally, I would like to thank Kaj for his patience in correcting our homework and the lengthy reports which even we are lazy to proof read at times. Thanks for being so enthusiastic in giving out the grades in the past week! Finally, thanks to the professor for being such a great story teller and for conveying the perfect story in connecting the concepts and also for bringing in guests to give us the sense of career changes, different fields Software development can lead to, their attitudes, etc. Hope to have a lecture by you soon!</t>
+  </si>
+  <si>
+    <t>Excited for break!</t>
   </si>
 </sst>
 </file>
@@ -2902,68 +2980,152 @@
         <v>165</v>
       </c>
     </row>
-    <row r="43" ht="15.5" customHeight="1">
-      <c r="A43" s="27"/>
-      <c r="B43" s="28"/>
-      <c r="C43" s="28"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="28"/>
-      <c r="F43" s="28"/>
-      <c r="G43" s="29"/>
-    </row>
-    <row r="44" ht="15.5" customHeight="1">
-      <c r="A44" s="30"/>
-      <c r="B44" s="31"/>
-      <c r="C44" s="31"/>
-      <c r="D44" s="31"/>
-      <c r="E44" s="31"/>
-      <c r="F44" s="31"/>
-      <c r="G44" s="32"/>
-    </row>
-    <row r="45" ht="15.5" customHeight="1">
-      <c r="A45" s="30"/>
-      <c r="B45" s="31"/>
-      <c r="C45" s="31"/>
-      <c r="D45" s="31"/>
-      <c r="E45" s="31"/>
-      <c r="F45" s="31"/>
-      <c r="G45" s="32"/>
-    </row>
-    <row r="46" ht="15.5" customHeight="1">
-      <c r="A46" s="30"/>
-      <c r="B46" s="31"/>
-      <c r="C46" s="31"/>
-      <c r="D46" s="31"/>
-      <c r="E46" s="31"/>
-      <c r="F46" s="31"/>
-      <c r="G46" s="32"/>
-    </row>
-    <row r="47" ht="15.5" customHeight="1">
-      <c r="A47" s="30"/>
-      <c r="B47" s="31"/>
-      <c r="C47" s="31"/>
-      <c r="D47" s="31"/>
-      <c r="E47" s="31"/>
-      <c r="F47" s="31"/>
-      <c r="G47" s="32"/>
-    </row>
-    <row r="48" ht="15.5" customHeight="1">
-      <c r="A48" s="30"/>
-      <c r="B48" s="31"/>
-      <c r="C48" s="31"/>
-      <c r="D48" s="31"/>
-      <c r="E48" s="31"/>
-      <c r="F48" s="31"/>
-      <c r="G48" s="32"/>
+    <row r="43" ht="352.65" customHeight="1">
+      <c r="A43" s="19">
+        <v>43895</v>
+      </c>
+      <c r="B43" t="s" s="20">
+        <v>14</v>
+      </c>
+      <c r="C43" t="s" s="20">
+        <v>21</v>
+      </c>
+      <c r="D43" t="s" s="20">
+        <v>166</v>
+      </c>
+      <c r="E43" t="s" s="20">
+        <v>167</v>
+      </c>
+      <c r="F43" t="s" s="20">
+        <v>168</v>
+      </c>
+      <c r="G43" t="s" s="21">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="44" ht="115.2" customHeight="1">
+      <c r="A44" s="19">
+        <v>43896</v>
+      </c>
+      <c r="B44" t="s" s="20">
+        <v>170</v>
+      </c>
+      <c r="C44" t="s" s="20">
+        <v>114</v>
+      </c>
+      <c r="D44" t="s" s="20">
+        <v>171</v>
+      </c>
+      <c r="E44" t="s" s="20">
+        <v>172</v>
+      </c>
+      <c r="F44" t="s" s="20">
+        <v>173</v>
+      </c>
+      <c r="G44" t="s" s="21">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="45" ht="221" customHeight="1">
+      <c r="A45" s="19">
+        <v>43902</v>
+      </c>
+      <c r="B45" t="s" s="20">
+        <v>14</v>
+      </c>
+      <c r="C45" t="s" s="20">
+        <v>21</v>
+      </c>
+      <c r="D45" t="s" s="20">
+        <v>175</v>
+      </c>
+      <c r="E45" t="s" s="20">
+        <v>176</v>
+      </c>
+      <c r="F45" t="s" s="20">
+        <v>177</v>
+      </c>
+      <c r="G45" t="s" s="21">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="46" ht="115" customHeight="1">
+      <c r="A46" s="19">
+        <v>43904</v>
+      </c>
+      <c r="B46" t="s" s="20">
+        <v>179</v>
+      </c>
+      <c r="C46" t="s" s="20">
+        <v>114</v>
+      </c>
+      <c r="D46" t="s" s="20">
+        <v>180</v>
+      </c>
+      <c r="E46" t="s" s="20">
+        <v>181</v>
+      </c>
+      <c r="F46" t="s" s="20">
+        <v>182</v>
+      </c>
+      <c r="G46" t="s" s="21">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="47" ht="145.3" customHeight="1">
+      <c r="A47" s="19">
+        <v>43905</v>
+      </c>
+      <c r="B47" t="s" s="20">
+        <v>170</v>
+      </c>
+      <c r="C47" t="s" s="20">
+        <v>114</v>
+      </c>
+      <c r="D47" t="s" s="20">
+        <v>184</v>
+      </c>
+      <c r="E47" t="s" s="20">
+        <v>185</v>
+      </c>
+      <c r="F47" t="s" s="20">
+        <v>186</v>
+      </c>
+      <c r="G47" t="s" s="21">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" ht="461.05" customHeight="1">
+      <c r="A48" s="19">
+        <v>43906</v>
+      </c>
+      <c r="B48" t="s" s="20">
+        <v>187</v>
+      </c>
+      <c r="C48" t="s" s="20">
+        <v>21</v>
+      </c>
+      <c r="D48" t="s" s="20">
+        <v>188</v>
+      </c>
+      <c r="E48" t="s" s="20">
+        <v>189</v>
+      </c>
+      <c r="F48" t="s" s="20">
+        <v>190</v>
+      </c>
+      <c r="G48" t="s" s="21">
+        <v>191</v>
+      </c>
     </row>
     <row r="49" ht="15.5" customHeight="1">
-      <c r="A49" s="30"/>
-      <c r="B49" s="31"/>
-      <c r="C49" s="31"/>
-      <c r="D49" s="31"/>
-      <c r="E49" s="31"/>
-      <c r="F49" s="31"/>
-      <c r="G49" s="32"/>
+      <c r="A49" s="27"/>
+      <c r="B49" s="28"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="28"/>
+      <c r="F49" s="28"/>
+      <c r="G49" s="29"/>
     </row>
     <row r="50" ht="15.5" customHeight="1">
       <c r="A50" s="30"/>

</xml_diff>